<commit_message>
final version lecture data 2
</commit_message>
<xml_diff>
--- a/Data-analyysiharjoitukset/Excel Data 2_valmis.xlsx
+++ b/Data-analyysiharjoitukset/Excel Data 2_valmis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hebpu\Code_KAMK\K25\JAMK\BusinessAnalytics_Resprictive\Data-analyysiharjoitukset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D154654-B9D8-4078-BF5F-6F5D45BFA0C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D87AF02B-1DFC-4DDF-8478-02A43E40C8D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" firstSheet="1" activeTab="6" xr2:uid="{C895F425-1013-47D7-A0DE-20E3812F0317}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" firstSheet="1" activeTab="7" xr2:uid="{C895F425-1013-47D7-A0DE-20E3812F0317}"/>
   </bookViews>
   <sheets>
     <sheet name="Tunnusluvut" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="Skenaarion yhteenveto" sheetId="12" r:id="rId7"/>
     <sheet name="Tavoitteen haku" sheetId="8" r:id="rId8"/>
     <sheet name="Ratkaisin" sheetId="9" r:id="rId9"/>
+    <sheet name="Vastausraportti 1" sheetId="13" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">Boxplot!$B$1</definedName>
@@ -32,43 +33,41 @@
     <definedName name="_xlchart.v1.5" hidden="1">Boxplot!$D$2:$D$13</definedName>
     <definedName name="_xlchart.v1.6" hidden="1">Histogrammi!$A$1</definedName>
     <definedName name="_xlchart.v1.7" hidden="1">Histogrammi!$A$2:$A$13</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Histogrammi!$A$1</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Histogrammi!$A$2:$A$13</definedName>
     <definedName name="Muut_muuttuvat">Skenaario!$E$7</definedName>
     <definedName name="Myyntihinta">Skenaario!$B$6</definedName>
     <definedName name="Myyntimäärä">Skenaario!$B$5</definedName>
     <definedName name="Palkat">Skenaario!$E$5</definedName>
     <definedName name="Raaka_aine">Skenaario!$E$6</definedName>
     <definedName name="Raakaaine">Skenaario!$E$6</definedName>
-    <definedName name="solver_adj" localSheetId="8" hidden="1">Ratkaisin!$F$7</definedName>
+    <definedName name="solver_adj" localSheetId="8" hidden="1">Ratkaisin!$B$2:$B$4</definedName>
     <definedName name="solver_cvg" localSheetId="8" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="8" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="8" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="8" hidden="1">1</definedName>
     <definedName name="solver_itr" localSheetId="8" hidden="1">2147483647</definedName>
-    <definedName name="solver_lhs1" localSheetId="8" hidden="1">Ratkaisin!$H$5</definedName>
-    <definedName name="solver_lhs2" localSheetId="8" hidden="1">Ratkaisin!$H$5</definedName>
-    <definedName name="solver_lhs3" localSheetId="8" hidden="1">Ratkaisin!$H$5</definedName>
-    <definedName name="solver_lhs4" localSheetId="8" hidden="1">Ratkaisin!$H$5</definedName>
+    <definedName name="solver_lhs1" localSheetId="8" hidden="1">Ratkaisin!$B$2:$B$4</definedName>
+    <definedName name="solver_lhs2" localSheetId="8" hidden="1">Ratkaisin!$B$2:$B$4</definedName>
+    <definedName name="solver_lhs3" localSheetId="8" hidden="1">Ratkaisin!$D$7</definedName>
+    <definedName name="solver_lhs4" localSheetId="8" hidden="1">Ratkaisin!$F$7</definedName>
     <definedName name="solver_mip" localSheetId="8" hidden="1">2147483647</definedName>
     <definedName name="solver_mni" localSheetId="8" hidden="1">30</definedName>
     <definedName name="solver_mrt" localSheetId="8" hidden="1">0.075</definedName>
     <definedName name="solver_msl" localSheetId="8" hidden="1">2</definedName>
     <definedName name="solver_neg" localSheetId="8" hidden="1">1</definedName>
     <definedName name="solver_nod" localSheetId="8" hidden="1">2147483647</definedName>
-    <definedName name="solver_num" localSheetId="8" hidden="1">0</definedName>
+    <definedName name="solver_num" localSheetId="8" hidden="1">4</definedName>
     <definedName name="solver_nwt" localSheetId="8" hidden="1">1</definedName>
-    <definedName name="solver_opt" localSheetId="8" hidden="1">Ratkaisin!$F$5</definedName>
+    <definedName name="solver_opt" localSheetId="8" hidden="1">Ratkaisin!$I$7</definedName>
     <definedName name="solver_pre" localSheetId="8" hidden="1">0.000001</definedName>
     <definedName name="solver_rbv" localSheetId="8" hidden="1">1</definedName>
-    <definedName name="solver_rel1" localSheetId="8" hidden="1">1</definedName>
-    <definedName name="solver_rel2" localSheetId="8" hidden="1">1</definedName>
+    <definedName name="solver_rel1" localSheetId="8" hidden="1">4</definedName>
+    <definedName name="solver_rel2" localSheetId="8" hidden="1">3</definedName>
     <definedName name="solver_rel3" localSheetId="8" hidden="1">1</definedName>
     <definedName name="solver_rel4" localSheetId="8" hidden="1">1</definedName>
-    <definedName name="solver_rhs1" localSheetId="8" hidden="1">300</definedName>
-    <definedName name="solver_rhs2" localSheetId="8" hidden="1">300</definedName>
-    <definedName name="solver_rhs3" localSheetId="8" hidden="1">300</definedName>
-    <definedName name="solver_rhs4" localSheetId="8" hidden="1">300</definedName>
+    <definedName name="solver_rhs1" localSheetId="8" hidden="1">"kokonaisluku"</definedName>
+    <definedName name="solver_rhs2" localSheetId="8" hidden="1">0</definedName>
+    <definedName name="solver_rhs3" localSheetId="8" hidden="1">3000</definedName>
+    <definedName name="solver_rhs4" localSheetId="8" hidden="1">1200</definedName>
     <definedName name="solver_rlx" localSheetId="8" hidden="1">2</definedName>
     <definedName name="solver_rsd" localSheetId="8" hidden="1">0</definedName>
     <definedName name="solver_scl" localSheetId="8" hidden="1">1</definedName>
@@ -137,7 +136,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="174">
   <si>
     <t>Kuukausi</t>
   </si>
@@ -527,6 +526,138 @@
   </si>
   <si>
     <t>Tulos</t>
+  </si>
+  <si>
+    <t>Microsoft Excel 16.0 Vastausraportti</t>
+  </si>
+  <si>
+    <t>Laskentataulukko: [Excel Data 2_valmis.xlsx]Ratkaisin</t>
+  </si>
+  <si>
+    <t>Raportti luotu: 17.4.2025 15.37.09</t>
+  </si>
+  <si>
+    <t>Tulos: Ratkaisin löysi ratkaisun, joka on kaikkien rajoitteiden ja optimaalisuusehtojen mukainen.</t>
+  </si>
+  <si>
+    <t>Ratkaisimen moduuli</t>
+  </si>
+  <si>
+    <t>Moduuli: GRG Nonlinear</t>
+  </si>
+  <si>
+    <t>Ratkaisuaika: 0,031 sekuntia</t>
+  </si>
+  <si>
+    <t>Iteraatiot: 0 Aliongelmat: 0</t>
+  </si>
+  <si>
+    <t>Ratkaisimen asetukset</t>
+  </si>
+  <si>
+    <t>Enimmäisaika Rajoittamaton,  Iteraatiot Rajoittamaton, Precision 0,000001, Automaattinen skaalaus</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Konvergenssi 0,0001, Populaation koko 100, Satunnaisalkuarvo 0, Derivaatat eteenpäin, Edellytä rajoja</t>
+  </si>
+  <si>
+    <t>Aliongelmia enintään Rajoittamaton, Kokonaislukuratkaisuja enintään Rajoittamaton, Kokonaislukutoleranssi 1%, Oleta ei-negatiiviseksi</t>
+  </si>
+  <si>
+    <t>Tavoitesolu (Suurin)</t>
+  </si>
+  <si>
+    <t>Solu</t>
+  </si>
+  <si>
+    <t>Nimi</t>
+  </si>
+  <si>
+    <t>Alkuperäinen arvo</t>
+  </si>
+  <si>
+    <t>Lopullinen arvo</t>
+  </si>
+  <si>
+    <t>Muuttujasolut</t>
+  </si>
+  <si>
+    <t>Kokonaisluku</t>
+  </si>
+  <si>
+    <t>Reunaehdot</t>
+  </si>
+  <si>
+    <t>Solun arvo</t>
+  </si>
+  <si>
+    <t>Kaava</t>
+  </si>
+  <si>
+    <t>Tila</t>
+  </si>
+  <si>
+    <t>Liukuma</t>
+  </si>
+  <si>
+    <t>$I$7</t>
+  </si>
+  <si>
+    <t>Yhteensä Tuotto/vrk</t>
+  </si>
+  <si>
+    <t>$B$2</t>
+  </si>
+  <si>
+    <t>Hiiri Kpl/vrk</t>
+  </si>
+  <si>
+    <t>$B$3</t>
+  </si>
+  <si>
+    <t>Näppäimistö Kpl/vrk</t>
+  </si>
+  <si>
+    <t>$B$4</t>
+  </si>
+  <si>
+    <t>Hiirimatto Kpl/vrk</t>
+  </si>
+  <si>
+    <t>$D$7</t>
+  </si>
+  <si>
+    <t>Yhteensä Kulut/vrk</t>
+  </si>
+  <si>
+    <t>$D$7&lt;=3000</t>
+  </si>
+  <si>
+    <t>Sitova</t>
+  </si>
+  <si>
+    <t>$F$7</t>
+  </si>
+  <si>
+    <t>Yhteensä Min/vrk</t>
+  </si>
+  <si>
+    <t>$F$7&lt;=1200</t>
+  </si>
+  <si>
+    <t>$B$2&gt;=0</t>
+  </si>
+  <si>
+    <t>Ei sitova</t>
+  </si>
+  <si>
+    <t>$B$3&gt;=0</t>
+  </si>
+  <si>
+    <t>$B$4&gt;=0</t>
+  </si>
+  <si>
+    <t>$B$2:$B$4=Kokonaisluku</t>
   </si>
 </sst>
 </file>
@@ -636,7 +767,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -661,8 +792,26 @@
         <bgColor indexed="7"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -730,12 +879,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="23"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="23"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="23"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="23"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="23"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -763,27 +943,25 @@
     <xf numFmtId="1" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -798,10 +976,20 @@
     <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normaali" xfId="0" builtinId="0"/>
@@ -1612,7 +1800,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.9</cx:f>
+        <cx:f>_xlchart.v1.7</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1623,7 +1811,7 @@
         <cx:series layoutId="clusteredColumn" uniqueId="{76E6BFCC-4858-4CAB-B5D9-F548836D90CF}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.8</cx:f>
+              <cx:f>_xlchart.v1.6</cx:f>
               <cx:v>Arvosana</cx:v>
             </cx:txData>
           </cx:tx>
@@ -3347,10 +3535,10 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="21"/>
+      <c r="E1" s="19"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -3359,8 +3547,6 @@
       <c r="B2" s="2">
         <v>5200</v>
       </c>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
@@ -3369,10 +3555,10 @@
       <c r="B3" s="2">
         <v>4800</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" t="s">
         <v>59</v>
       </c>
-      <c r="E3" s="17">
+      <c r="E3">
         <v>5741.666666666667</v>
       </c>
     </row>
@@ -3383,10 +3569,10 @@
       <c r="B4" s="2">
         <v>6100</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="D4" t="s">
         <v>60</v>
       </c>
-      <c r="E4" s="17">
+      <c r="E4">
         <v>267.83597799980356</v>
       </c>
     </row>
@@ -3397,10 +3583,10 @@
       <c r="B5" s="2">
         <v>4700</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" t="s">
         <v>61</v>
       </c>
-      <c r="E5" s="17">
+      <c r="E5">
         <v>5550</v>
       </c>
     </row>
@@ -3411,10 +3597,10 @@
       <c r="B6" s="2">
         <v>6500</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="D6" t="s">
         <v>62</v>
       </c>
-      <c r="E6" s="17">
+      <c r="E6">
         <v>4900</v>
       </c>
     </row>
@@ -3425,10 +3611,10 @@
       <c r="B7" s="2">
         <v>5300</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="D7" t="s">
         <v>63</v>
       </c>
-      <c r="E7" s="17">
+      <c r="E7">
         <v>927.81104398111961</v>
       </c>
     </row>
@@ -3439,10 +3625,10 @@
       <c r="B8" s="2">
         <v>4900</v>
       </c>
-      <c r="D8" s="17" t="s">
+      <c r="D8" t="s">
         <v>64</v>
       </c>
-      <c r="E8" s="17">
+      <c r="E8">
         <v>860833.33333333512</v>
       </c>
     </row>
@@ -3453,10 +3639,10 @@
       <c r="B9" s="2">
         <v>7000</v>
       </c>
-      <c r="D9" s="17" t="s">
+      <c r="D9" t="s">
         <v>65</v>
       </c>
-      <c r="E9" s="17">
+      <c r="E9">
         <v>-0.72698599988976031</v>
       </c>
     </row>
@@ -3467,10 +3653,10 @@
       <c r="B10" s="2">
         <v>5800</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="D10" t="s">
         <v>66</v>
       </c>
-      <c r="E10" s="17">
+      <c r="E10">
         <v>0.6289137864030977</v>
       </c>
     </row>
@@ -3481,10 +3667,10 @@
       <c r="B11" s="2">
         <v>6200</v>
       </c>
-      <c r="D11" s="17" t="s">
+      <c r="D11" t="s">
         <v>67</v>
       </c>
-      <c r="E11" s="17">
+      <c r="E11">
         <v>2800</v>
       </c>
     </row>
@@ -3495,10 +3681,10 @@
       <c r="B12" s="2">
         <v>4900</v>
       </c>
-      <c r="D12" s="17" t="s">
+      <c r="D12" t="s">
         <v>68</v>
       </c>
-      <c r="E12" s="17">
+      <c r="E12">
         <v>4700</v>
       </c>
     </row>
@@ -3509,44 +3695,370 @@
       <c r="B13" s="2">
         <v>7500</v>
       </c>
-      <c r="D13" s="17" t="s">
+      <c r="D13" t="s">
         <v>69</v>
       </c>
-      <c r="E13" s="17">
+      <c r="E13">
         <v>7500</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D14" s="17" t="s">
+      <c r="D14" t="s">
         <v>70</v>
       </c>
-      <c r="E14" s="17">
+      <c r="E14">
         <v>68900</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D15" s="17" t="s">
+      <c r="D15" t="s">
         <v>71</v>
       </c>
-      <c r="E15" s="17">
+      <c r="E15">
         <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D16" s="17" t="s">
+      <c r="D16" t="s">
         <v>72</v>
       </c>
-      <c r="E16" s="17">
+      <c r="E16">
         <v>6500</v>
       </c>
     </row>
     <row r="17" spans="4:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D17" s="18" t="s">
+      <c r="D17" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="E17" s="18">
+      <c r="E17" s="15">
         <v>4900</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFD1CF5A-4067-424E-80FC-B44BB3DD8761}">
+  <dimension ref="A1:G33"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="2.33203125" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="20" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="20" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="20" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="20" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="20" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="20"/>
+      <c r="B6" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="20"/>
+      <c r="B7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="20"/>
+      <c r="B8" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="20" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="36" t="s">
+        <v>143</v>
+      </c>
+      <c r="C15" s="36" t="s">
+        <v>144</v>
+      </c>
+      <c r="D15" s="36" t="s">
+        <v>145</v>
+      </c>
+      <c r="E15" s="36" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="35" t="s">
+        <v>154</v>
+      </c>
+      <c r="C16" s="35" t="s">
+        <v>155</v>
+      </c>
+      <c r="D16" s="38">
+        <v>1320</v>
+      </c>
+      <c r="E16" s="38">
+        <v>1320</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="36" t="s">
+        <v>143</v>
+      </c>
+      <c r="C20" s="36" t="s">
+        <v>144</v>
+      </c>
+      <c r="D20" s="36" t="s">
+        <v>145</v>
+      </c>
+      <c r="E20" s="36" t="s">
+        <v>146</v>
+      </c>
+      <c r="F20" s="36" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B21" s="37" t="s">
+        <v>156</v>
+      </c>
+      <c r="C21" s="37" t="s">
+        <v>157</v>
+      </c>
+      <c r="D21" s="39">
+        <v>20</v>
+      </c>
+      <c r="E21" s="39">
+        <v>20</v>
+      </c>
+      <c r="F21" s="37" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B22" s="37" t="s">
+        <v>158</v>
+      </c>
+      <c r="C22" s="37" t="s">
+        <v>159</v>
+      </c>
+      <c r="D22" s="39">
+        <v>200</v>
+      </c>
+      <c r="E22" s="39">
+        <v>200</v>
+      </c>
+      <c r="F22" s="37" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="35" t="s">
+        <v>160</v>
+      </c>
+      <c r="C23" s="35" t="s">
+        <v>161</v>
+      </c>
+      <c r="D23" s="38">
+        <v>0</v>
+      </c>
+      <c r="E23" s="38">
+        <v>0</v>
+      </c>
+      <c r="F23" s="35" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B27" s="36" t="s">
+        <v>143</v>
+      </c>
+      <c r="C27" s="36" t="s">
+        <v>144</v>
+      </c>
+      <c r="D27" s="36" t="s">
+        <v>150</v>
+      </c>
+      <c r="E27" s="36" t="s">
+        <v>151</v>
+      </c>
+      <c r="F27" s="36" t="s">
+        <v>152</v>
+      </c>
+      <c r="G27" s="36" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B28" s="37" t="s">
+        <v>162</v>
+      </c>
+      <c r="C28" s="37" t="s">
+        <v>163</v>
+      </c>
+      <c r="D28" s="39">
+        <v>3000</v>
+      </c>
+      <c r="E28" s="37" t="s">
+        <v>164</v>
+      </c>
+      <c r="F28" s="37" t="s">
+        <v>165</v>
+      </c>
+      <c r="G28" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B29" s="37" t="s">
+        <v>166</v>
+      </c>
+      <c r="C29" s="37" t="s">
+        <v>167</v>
+      </c>
+      <c r="D29" s="39">
+        <v>1200</v>
+      </c>
+      <c r="E29" s="37" t="s">
+        <v>168</v>
+      </c>
+      <c r="F29" s="37" t="s">
+        <v>165</v>
+      </c>
+      <c r="G29" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B30" s="37" t="s">
+        <v>156</v>
+      </c>
+      <c r="C30" s="37" t="s">
+        <v>157</v>
+      </c>
+      <c r="D30" s="39">
+        <v>20</v>
+      </c>
+      <c r="E30" s="37" t="s">
+        <v>169</v>
+      </c>
+      <c r="F30" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="G30" s="39">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B31" s="37" t="s">
+        <v>158</v>
+      </c>
+      <c r="C31" s="37" t="s">
+        <v>159</v>
+      </c>
+      <c r="D31" s="39">
+        <v>200</v>
+      </c>
+      <c r="E31" s="37" t="s">
+        <v>171</v>
+      </c>
+      <c r="F31" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="G31" s="39">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B32" s="37" t="s">
+        <v>160</v>
+      </c>
+      <c r="C32" s="37" t="s">
+        <v>161</v>
+      </c>
+      <c r="D32" s="39">
+        <v>0</v>
+      </c>
+      <c r="E32" s="37" t="s">
+        <v>172</v>
+      </c>
+      <c r="F32" s="37" t="s">
+        <v>165</v>
+      </c>
+      <c r="G32" s="39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B33" s="35" t="s">
+        <v>173</v>
+      </c>
+      <c r="C33" s="35"/>
+      <c r="D33" s="35"/>
+      <c r="E33" s="35"/>
+      <c r="F33" s="35"/>
+      <c r="G33" s="35"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3602,14 +4114,14 @@
       <c r="D2" s="2">
         <v>150</v>
       </c>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20" t="s">
+      <c r="F2" s="18"/>
+      <c r="G2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="20" t="s">
+      <c r="H2" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="20" t="s">
+      <c r="I2" s="18" t="s">
         <v>15</v>
       </c>
     </row>
@@ -3626,14 +4138,12 @@
       <c r="D3" s="2">
         <v>140</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="F3" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="17">
+      <c r="G3">
         <v>1</v>
       </c>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
@@ -3648,16 +4158,15 @@
       <c r="D4" s="2">
         <v>160</v>
       </c>
-      <c r="F4" s="17" t="s">
+      <c r="F4" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="17">
+      <c r="G4">
         <v>0.9940313266134323</v>
       </c>
-      <c r="H4" s="17">
+      <c r="H4">
         <v>1</v>
       </c>
-      <c r="I4" s="17"/>
     </row>
     <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
@@ -3672,16 +4181,16 @@
       <c r="D5" s="2">
         <v>130</v>
       </c>
-      <c r="F5" s="18" t="s">
+      <c r="F5" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="18">
+      <c r="G5" s="15">
         <v>0.98568636408650157</v>
       </c>
-      <c r="H5" s="18">
+      <c r="H5" s="15">
         <v>0.98859079906026548</v>
       </c>
-      <c r="I5" s="18">
+      <c r="I5" s="15">
         <v>1</v>
       </c>
     </row>
@@ -3892,10 +4401,10 @@
       <c r="D4" s="2">
         <v>160</v>
       </c>
-      <c r="H4" s="21" t="s">
+      <c r="H4" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="I4" s="21"/>
+      <c r="I4" s="19"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
@@ -3910,10 +4419,10 @@
       <c r="D5" s="2">
         <v>130</v>
       </c>
-      <c r="H5" s="17" t="s">
+      <c r="H5" t="s">
         <v>78</v>
       </c>
-      <c r="I5" s="17">
+      <c r="I5">
         <v>0.99423032529259603</v>
       </c>
       <c r="J5" t="s">
@@ -3933,10 +4442,10 @@
       <c r="D6" s="2">
         <v>170</v>
       </c>
-      <c r="H6" s="17" t="s">
+      <c r="H6" t="s">
         <v>79</v>
       </c>
-      <c r="I6" s="22">
+      <c r="I6" s="20">
         <v>0.9884939397314213</v>
       </c>
       <c r="J6" t="s">
@@ -3956,10 +4465,10 @@
       <c r="D7" s="2">
         <v>150</v>
       </c>
-      <c r="H7" s="17" t="s">
+      <c r="H7" t="s">
         <v>80</v>
       </c>
-      <c r="I7" s="17">
+      <c r="I7">
         <v>0.98593703744951489</v>
       </c>
       <c r="J7" t="s">
@@ -3979,10 +4488,10 @@
       <c r="D8" s="2">
         <v>140</v>
       </c>
-      <c r="H8" s="17" t="s">
+      <c r="H8" t="s">
         <v>60</v>
       </c>
-      <c r="I8" s="22">
+      <c r="I8" s="20">
         <v>110.02666462669758</v>
       </c>
       <c r="J8" t="s">
@@ -4002,10 +4511,10 @@
       <c r="D9" s="2">
         <v>180</v>
       </c>
-      <c r="H9" s="18" t="s">
+      <c r="H9" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="I9" s="18">
+      <c r="I9" s="15">
         <v>12</v>
       </c>
     </row>
@@ -4059,20 +4568,20 @@
       <c r="D12" s="2">
         <v>140</v>
       </c>
-      <c r="H12" s="20"/>
-      <c r="I12" s="20" t="s">
+      <c r="H12" s="18"/>
+      <c r="I12" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="J12" s="20" t="s">
+      <c r="J12" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="K12" s="20" t="s">
+      <c r="K12" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="L12" s="23" t="s">
+      <c r="L12" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="M12" s="23" t="s">
+      <c r="M12" s="21" t="s">
         <v>90</v>
       </c>
     </row>
@@ -4089,167 +4598,165 @@
       <c r="D13" s="2">
         <v>190</v>
       </c>
-      <c r="H13" s="17" t="s">
+      <c r="H13" t="s">
         <v>83</v>
       </c>
-      <c r="I13" s="17">
+      <c r="I13">
         <v>2</v>
       </c>
-      <c r="J13" s="17">
+      <c r="J13">
         <v>9360213.8643067833</v>
       </c>
-      <c r="K13" s="17">
+      <c r="K13">
         <v>4680106.9321533917</v>
       </c>
-      <c r="L13" s="17">
+      <c r="L13">
         <v>386.59824692026507</v>
       </c>
-      <c r="M13" s="17">
+      <c r="M13">
         <v>1.8800521682178645E-9</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="H14" s="17" t="s">
+      <c r="H14" t="s">
         <v>84</v>
       </c>
-      <c r="I14" s="17">
+      <c r="I14">
         <v>9</v>
       </c>
-      <c r="J14" s="17">
+      <c r="J14">
         <v>108952.80235988206</v>
       </c>
-      <c r="K14" s="17">
+      <c r="K14">
         <v>12105.866928875785</v>
       </c>
-      <c r="L14" s="17"/>
-      <c r="M14" s="17"/>
     </row>
     <row r="15" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="H15" s="18" t="s">
+      <c r="H15" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="I15" s="18">
+      <c r="I15" s="15">
         <v>11</v>
       </c>
-      <c r="J15" s="18">
+      <c r="J15" s="15">
         <v>9469166.666666666</v>
       </c>
-      <c r="K15" s="18"/>
-      <c r="L15" s="18"/>
-      <c r="M15" s="18"/>
+      <c r="K15" s="15"/>
+      <c r="L15" s="15"/>
+      <c r="M15" s="15"/>
     </row>
     <row r="16" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="17" spans="8:16" x14ac:dyDescent="0.3">
-      <c r="H17" s="20"/>
-      <c r="I17" s="20" t="s">
+      <c r="H17" s="18"/>
+      <c r="I17" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="J17" s="20" t="s">
+      <c r="J17" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="K17" s="20" t="s">
+      <c r="K17" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="L17" s="20" t="s">
+      <c r="L17" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="M17" s="20" t="s">
+      <c r="M17" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="N17" s="20" t="s">
+      <c r="N17" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="O17" s="20" t="s">
+      <c r="O17" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="P17" s="20" t="s">
+      <c r="P17" s="18" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="18" spans="8:16" x14ac:dyDescent="0.3">
-      <c r="H18" s="17" t="s">
+      <c r="H18" t="s">
         <v>85</v>
       </c>
-      <c r="I18" s="17">
+      <c r="I18">
         <v>-656.48967551622468</v>
       </c>
-      <c r="J18" s="17">
+      <c r="J18">
         <v>490.72793330688984</v>
       </c>
-      <c r="K18" s="17">
+      <c r="K18">
         <v>-1.3377874601356172</v>
       </c>
-      <c r="L18" s="17">
+      <c r="L18">
         <v>0.21378456637116278</v>
       </c>
-      <c r="M18" s="17">
+      <c r="M18">
         <v>-1766.5933848315656</v>
       </c>
-      <c r="N18" s="17">
+      <c r="N18">
         <v>453.61403379911621</v>
       </c>
-      <c r="O18" s="17">
+      <c r="O18">
         <v>-1766.5933848315656</v>
       </c>
-      <c r="P18" s="17">
+      <c r="P18">
         <v>453.61403379911621</v>
       </c>
     </row>
     <row r="19" spans="8:16" x14ac:dyDescent="0.3">
-      <c r="H19" s="17" t="s">
+      <c r="H19" t="s">
         <v>14</v>
       </c>
-      <c r="I19" s="17">
+      <c r="I19">
         <v>16.12094395280236</v>
       </c>
-      <c r="J19" s="17">
+      <c r="J19">
         <v>4.4317927583257228</v>
       </c>
-      <c r="K19" s="17">
+      <c r="K19">
         <v>3.6375671950176334</v>
       </c>
-      <c r="L19" s="17">
+      <c r="L19">
         <v>5.4213738732340937E-3</v>
       </c>
-      <c r="M19" s="17">
+      <c r="M19">
         <v>6.09553222051861</v>
       </c>
-      <c r="N19" s="17">
+      <c r="N19">
         <v>26.14635568508611</v>
       </c>
-      <c r="O19" s="17">
+      <c r="O19">
         <v>6.09553222051861</v>
       </c>
-      <c r="P19" s="17">
+      <c r="P19">
         <v>26.14635568508611</v>
       </c>
     </row>
     <row r="20" spans="8:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="H20" s="18" t="s">
+      <c r="H20" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="I20" s="18">
+      <c r="I20" s="15">
         <v>6.7109144542772867</v>
       </c>
-      <c r="J20" s="18">
+      <c r="J20" s="15">
         <v>12.063182697775412</v>
       </c>
-      <c r="K20" s="18">
+      <c r="K20" s="15">
         <v>0.55631375420641316</v>
       </c>
-      <c r="L20" s="18">
+      <c r="L20" s="15">
         <v>0.59155722947273737</v>
       </c>
-      <c r="M20" s="18">
+      <c r="M20" s="15">
         <v>-20.577900691638739</v>
       </c>
-      <c r="N20" s="18">
+      <c r="N20" s="15">
         <v>33.999729600193312</v>
       </c>
-      <c r="O20" s="18">
+      <c r="O20" s="15">
         <v>-20.577900691638739</v>
       </c>
-      <c r="P20" s="18">
+      <c r="P20" s="15">
         <v>33.999729600193312</v>
       </c>
     </row>
@@ -4260,145 +4767,145 @@
     </row>
     <row r="25" spans="8:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="26" spans="8:16" x14ac:dyDescent="0.3">
-      <c r="H26" s="20" t="s">
+      <c r="H26" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="I26" s="20" t="s">
+      <c r="I26" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="J26" s="20" t="s">
+      <c r="J26" s="18" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="27" spans="8:16" x14ac:dyDescent="0.3">
-      <c r="H27" s="17">
+      <c r="H27">
         <v>1</v>
       </c>
-      <c r="I27" s="17">
+      <c r="I27">
         <v>5186.4306784660766</v>
       </c>
-      <c r="J27" s="17">
+      <c r="J27">
         <v>13.569321533923357</v>
       </c>
     </row>
     <row r="28" spans="8:16" x14ac:dyDescent="0.3">
-      <c r="H28" s="17">
+      <c r="H28">
         <v>2</v>
       </c>
-      <c r="I28" s="17">
+      <c r="I28">
         <v>4796.9026548672564</v>
       </c>
-      <c r="J28" s="17">
+      <c r="J28">
         <v>3.0973451327436123</v>
       </c>
     </row>
     <row r="29" spans="8:16" x14ac:dyDescent="0.3">
-      <c r="H29" s="17">
+      <c r="H29">
         <v>3</v>
       </c>
-      <c r="I29" s="17">
+      <c r="I29">
         <v>6059.5870206489672</v>
       </c>
-      <c r="J29" s="17">
+      <c r="J29">
         <v>40.412979351032845</v>
       </c>
     </row>
     <row r="30" spans="8:16" x14ac:dyDescent="0.3">
-      <c r="H30" s="17">
+      <c r="H30">
         <v>4</v>
       </c>
-      <c r="I30" s="17">
+      <c r="I30">
         <v>4568.5840707964599</v>
       </c>
-      <c r="J30" s="17">
+      <c r="J30">
         <v>131.41592920354014</v>
       </c>
     </row>
     <row r="31" spans="8:16" x14ac:dyDescent="0.3">
-      <c r="H31" s="17">
+      <c r="H31">
         <v>5</v>
       </c>
-      <c r="I31" s="17">
+      <c r="I31">
         <v>6449.1150442477874</v>
       </c>
-      <c r="J31" s="17">
+      <c r="J31">
         <v>50.884955752212591</v>
       </c>
     </row>
     <row r="32" spans="8:16" x14ac:dyDescent="0.3">
-      <c r="H32" s="17">
+      <c r="H32">
         <v>6</v>
       </c>
-      <c r="I32" s="17">
+      <c r="I32">
         <v>5508.8495575221241</v>
       </c>
-      <c r="J32" s="17">
+      <c r="J32">
         <v>-208.84955752212409</v>
       </c>
     </row>
     <row r="33" spans="7:13" x14ac:dyDescent="0.3">
-      <c r="H33" s="17">
+      <c r="H33">
         <v>7</v>
       </c>
-      <c r="I33" s="17">
+      <c r="I33">
         <v>4958.1120943952801</v>
       </c>
-      <c r="J33" s="17">
+      <c r="J33">
         <v>-58.11209439528011</v>
       </c>
     </row>
     <row r="34" spans="7:13" x14ac:dyDescent="0.3">
-      <c r="H34" s="17">
+      <c r="H34">
         <v>8</v>
       </c>
-      <c r="I34" s="17">
+      <c r="I34">
         <v>6999.8525073746314</v>
       </c>
-      <c r="J34" s="17">
+      <c r="J34">
         <v>0.14749262536861352</v>
       </c>
     </row>
     <row r="35" spans="7:13" x14ac:dyDescent="0.3">
-      <c r="H35" s="17">
+      <c r="H35">
         <v>9</v>
       </c>
-      <c r="I35" s="17">
+      <c r="I35">
         <v>5898.3775811209434</v>
       </c>
-      <c r="J35" s="17">
+      <c r="J35">
         <v>-98.377581120943432</v>
       </c>
     </row>
     <row r="36" spans="7:13" x14ac:dyDescent="0.3">
-      <c r="H36" s="17">
+      <c r="H36">
         <v>10</v>
       </c>
-      <c r="I36" s="17">
+      <c r="I36">
         <v>6287.9056047197637</v>
       </c>
-      <c r="J36" s="17">
+      <c r="J36">
         <v>-87.905604719763687</v>
       </c>
     </row>
     <row r="37" spans="7:13" x14ac:dyDescent="0.3">
-      <c r="H37" s="17">
+      <c r="H37">
         <v>11</v>
       </c>
-      <c r="I37" s="17">
+      <c r="I37">
         <v>4796.9026548672564</v>
       </c>
-      <c r="J37" s="17">
+      <c r="J37">
         <v>103.09734513274361</v>
       </c>
     </row>
     <row r="38" spans="7:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="H38" s="18">
+      <c r="H38" s="15">
         <v>12</v>
       </c>
-      <c r="I38" s="18">
+      <c r="I38" s="15">
         <v>7389.3805309734507</v>
       </c>
-      <c r="J38" s="18">
+      <c r="J38" s="15">
         <v>110.61946902654927</v>
       </c>
     </row>
@@ -5100,7 +5607,7 @@
   </sheetPr>
   <dimension ref="B1:F15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
   <cols>
@@ -5110,143 +5617,142 @@
   <sheetData>
     <row r="1" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
     </row>
     <row r="3" spans="2:6" ht="15.6" collapsed="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="31" t="s">
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="29" t="s">
         <v>119</v>
       </c>
-      <c r="E3" s="31" t="s">
+      <c r="E3" s="29" t="s">
         <v>114</v>
       </c>
-      <c r="F3" s="31" t="s">
+      <c r="F3" s="29" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="21.6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="33" t="s">
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="E4" s="31" t="s">
         <v>115</v>
       </c>
-      <c r="F4" s="33" t="s">
+      <c r="F4" s="31" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="26" t="s">
         <v>118</v>
       </c>
-      <c r="C5" s="28"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
     </row>
     <row r="6" spans="2:6" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="27"/>
-      <c r="C6" s="27" t="s">
+      <c r="B6" s="25"/>
+      <c r="C6" s="25" t="s">
         <v>124</v>
       </c>
-      <c r="D6" s="17">
+      <c r="D6">
         <v>17000</v>
       </c>
-      <c r="E6" s="32">
+      <c r="E6" s="30">
         <v>17000</v>
       </c>
-      <c r="F6" s="32">
+      <c r="F6" s="30">
         <v>12500</v>
       </c>
     </row>
     <row r="7" spans="2:6" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="27"/>
-      <c r="C7" s="27" t="s">
+      <c r="B7" s="25"/>
+      <c r="C7" s="25" t="s">
         <v>125</v>
       </c>
-      <c r="D7" s="17">
+      <c r="D7">
         <v>105</v>
       </c>
-      <c r="E7" s="32">
+      <c r="E7" s="30">
         <v>105</v>
       </c>
-      <c r="F7" s="32">
+      <c r="F7" s="30">
         <v>125</v>
       </c>
     </row>
     <row r="8" spans="2:6" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="27"/>
-      <c r="C8" s="27" t="s">
+      <c r="B8" s="25"/>
+      <c r="C8" s="25" t="s">
         <v>126</v>
       </c>
-      <c r="D8" s="17">
+      <c r="D8">
         <v>27</v>
       </c>
-      <c r="E8" s="32">
+      <c r="E8" s="30">
         <v>27</v>
       </c>
-      <c r="F8" s="32">
+      <c r="F8" s="30">
         <v>27</v>
       </c>
     </row>
     <row r="9" spans="2:6" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="27"/>
-      <c r="C9" s="27" t="s">
+      <c r="B9" s="25"/>
+      <c r="C9" s="25" t="s">
         <v>127</v>
       </c>
-      <c r="D9" s="17">
+      <c r="D9">
         <v>32</v>
       </c>
-      <c r="E9" s="32">
+      <c r="E9" s="30">
         <v>32</v>
       </c>
-      <c r="F9" s="32">
+      <c r="F9" s="30">
         <v>32</v>
       </c>
     </row>
     <row r="10" spans="2:6" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="27"/>
-      <c r="C10" s="27" t="s">
+      <c r="B10" s="25"/>
+      <c r="C10" s="25" t="s">
         <v>128</v>
       </c>
-      <c r="D10" s="17">
+      <c r="D10">
         <v>5</v>
       </c>
-      <c r="E10" s="32">
+      <c r="E10" s="30">
         <v>5</v>
       </c>
-      <c r="F10" s="32">
+      <c r="F10" s="30">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="C11" s="28"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
     </row>
     <row r="12" spans="2:6" ht="15" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="29"/>
-      <c r="C12" s="29" t="s">
+      <c r="B12" s="27"/>
+      <c r="C12" s="27" t="s">
         <v>129</v>
       </c>
-      <c r="D12" s="24">
+      <c r="D12" s="22">
         <v>279955.86875306698</v>
       </c>
-      <c r="E12" s="24">
+      <c r="E12" s="22">
         <v>279955.86875306698</v>
       </c>
-      <c r="F12" s="24">
+      <c r="F12" s="22">
         <v>380889.60241872701</v>
       </c>
     </row>
@@ -5274,7 +5780,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6648D494-6434-46A1-8E6C-C252E72345D0}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
@@ -5386,44 +5892,40 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView zoomScale="109" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.21875" customWidth="1"/>
-    <col min="3" max="3" width="15.88671875" customWidth="1"/>
-    <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="13.44140625" customWidth="1"/>
-    <col min="6" max="6" width="15.21875" customWidth="1"/>
+    <col min="1" max="9" width="17.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="32" t="s">
         <v>33</v>
       </c>
     </row>
@@ -5432,32 +5934,32 @@
         <v>34</v>
       </c>
       <c r="B2">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C2">
         <v>10</v>
       </c>
       <c r="D2">
         <f>B2*C2</f>
-        <v>50</v>
+        <v>200</v>
       </c>
       <c r="E2">
         <v>10</v>
       </c>
       <c r="F2">
         <f>B2*10</f>
-        <v>50</v>
+        <v>200</v>
       </c>
       <c r="G2">
         <v>16</v>
       </c>
       <c r="H2">
         <f>B2*G2</f>
-        <v>80</v>
+        <v>320</v>
       </c>
       <c r="I2">
         <f>H2-D2</f>
-        <v>30</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -5465,32 +5967,32 @@
         <v>35</v>
       </c>
       <c r="B3">
-        <v>5</v>
+        <v>200</v>
       </c>
       <c r="C3">
         <v>14</v>
       </c>
       <c r="D3">
         <f>B3*C3</f>
-        <v>70</v>
+        <v>2800</v>
       </c>
       <c r="E3">
         <v>5</v>
       </c>
       <c r="F3">
         <f>B3*5</f>
-        <v>25</v>
+        <v>1000</v>
       </c>
       <c r="G3">
         <v>20</v>
       </c>
       <c r="H3">
         <f>B3*G3</f>
-        <v>100</v>
+        <v>4000</v>
       </c>
       <c r="I3">
         <f>H3-D3</f>
-        <v>30</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -5498,49 +6000,49 @@
         <v>36</v>
       </c>
       <c r="B4">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4">
         <f>B4*C4</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E4">
         <v>6</v>
       </c>
       <c r="F4">
         <f>B4*6</f>
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="G4">
         <v>2</v>
       </c>
       <c r="H4">
         <f>B4*G4</f>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="I4">
         <f>H4-D4</f>
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>18</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="33">
         <f>SUM(D2:D4)</f>
-        <v>125</v>
-      </c>
-      <c r="F7">
+        <v>3000</v>
+      </c>
+      <c r="F7" s="33">
         <f>SUM(F2:F4)</f>
-        <v>105</v>
-      </c>
-      <c r="I7">
+        <v>1200</v>
+      </c>
+      <c r="I7" s="34">
         <f>SUM(I2:I6)</f>
-        <v>65</v>
+        <v>1320</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>